<commit_message>
update course list and research experience
</commit_message>
<xml_diff>
--- a/images/chenda-courselist.xlsx
+++ b/images/chenda-courselist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duanchenda/Desktop/申请/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D55BE-B563-0A43-A56A-92DCCDD396D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0B7252-0102-E444-AB8F-47468D30D0E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="23780" windowHeight="16080" xr2:uid="{B49318F0-E753-F447-8326-ABA88061BE08}"/>
+    <workbookView xWindow="400" yWindow="500" windowWidth="23780" windowHeight="16080" xr2:uid="{B49318F0-E753-F447-8326-ABA88061BE08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="110">
   <si>
     <t xml:space="preserve">Class ID </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,14 +303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CSM146</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Introduction to Machine Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Computer Network Fundamentals</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -319,22 +311,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CS133</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parallel and Distributed Computing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CS136</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Introduction to Computer Security</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Physics1b</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -442,14 +418,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Currently Taking</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Planning to take</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Course name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -479,6 +447,30 @@
   </si>
   <si>
     <t>CS/Math Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRP199</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Currently taking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECE188</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secure Computing Systems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03/2022</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -875,7 +867,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -893,11 +885,11 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -910,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -922,13 +914,13 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>2</v>
@@ -940,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -963,16 +955,16 @@
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>16</v>
@@ -1001,16 +993,16 @@
         <v>4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>16</v>
@@ -1039,16 +1031,16 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>12</v>
@@ -1077,16 +1069,16 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>12</v>
@@ -1115,16 +1107,16 @@
         <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>16</v>
@@ -1153,19 +1145,19 @@
         <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M8" s="1">
         <v>2</v>
@@ -1194,7 +1186,7 @@
         <v>37</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M9" s="1">
         <v>2</v>
@@ -1226,7 +1218,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M10" s="1">
         <v>1</v>
@@ -1251,12 +1243,20 @@
       <c r="F11" s="1">
         <v>4</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
@@ -1278,16 +1278,16 @@
         <v>4</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>12</v>
@@ -1316,16 +1316,16 @@
         <v>4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>12</v>
@@ -1354,16 +1354,16 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>16</v>
@@ -1673,8 +1673,23 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="2" t="s">
-        <v>102</v>
+      <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1685,16 +1700,19 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F28" s="1">
         <v>4</v>
@@ -1711,15 +1729,17 @@
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F29" s="1">
         <v>4</v>
       </c>
@@ -1732,18 +1752,20 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F30" s="1">
         <v>4</v>
       </c>
@@ -1755,22 +1777,6 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1">
-        <v>4</v>
-      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1790,7 +1796,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1811,12 +1817,16 @@
       <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1826,14 +1836,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1845,16 +1857,10 @@
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1865,16 +1871,10 @@
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>

</xml_diff>